<commit_message>
Salvataggio Dati fine Tostatura OK
</commit_message>
<xml_diff>
--- a/Tostatura/Doc/DataMemory.xlsx
+++ b/Tostatura/Doc/DataMemory.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>Data Memory Progetto Tostatura</t>
   </si>
@@ -132,28 +132,25 @@
     <t>5023 - 5032</t>
   </si>
   <si>
-    <t>5034 - 5053</t>
-  </si>
-  <si>
     <t>Lunghezza</t>
   </si>
   <si>
     <t>3009 - 3016</t>
   </si>
   <si>
-    <t>Lotto Tostatura :</t>
-  </si>
-  <si>
-    <t>Giorno Giuliano</t>
-  </si>
-  <si>
-    <t>Codice Finito</t>
-  </si>
-  <si>
-    <t>Codice Grezzo</t>
-  </si>
-  <si>
-    <t>Codice Operatore</t>
+    <t>6001 - 6010</t>
+  </si>
+  <si>
+    <t>Data Allarme</t>
+  </si>
+  <si>
+    <t>valvola</t>
+  </si>
+  <si>
+    <t>apertura_valvola</t>
+  </si>
+  <si>
+    <t>5034 - 5043</t>
   </si>
 </sst>
 </file>
@@ -275,7 +272,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -283,9 +280,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,6 +323,25 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -638,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,101 +671,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>2990</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>2991</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>2992</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>2993</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <v>2994</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7">
+      <c r="A3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -760,309 +773,350 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>3000</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="10">
+        <v>3017</v>
+      </c>
+      <c r="F7" s="10">
+        <v>3018</v>
+      </c>
+      <c r="G7" s="10">
+        <v>3019</v>
+      </c>
+      <c r="H7" s="10">
+        <v>3020</v>
+      </c>
+      <c r="I7" s="10">
+        <v>3021</v>
+      </c>
+      <c r="J7" s="10">
+        <v>3022</v>
+      </c>
+      <c r="K7" s="10">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="9">
+        <v>5000</v>
+      </c>
+      <c r="C12" s="10">
+        <v>5001</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="10">
+        <v>5012</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="10">
+        <v>5033</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
+        <v>10</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>10</v>
+      </c>
+      <c r="G13" s="6">
+        <v>10</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1</v>
+      </c>
+      <c r="I13" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="9">
+        <v>6000</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="11">
-        <v>3017</v>
-      </c>
-      <c r="F7" s="11">
-        <v>3018</v>
-      </c>
-      <c r="G7" s="11">
-        <v>3019</v>
-      </c>
-      <c r="H7" s="11">
-        <v>3020</v>
-      </c>
-      <c r="I7" s="11">
-        <v>3021</v>
-      </c>
-      <c r="J7" s="11">
-        <v>3022</v>
-      </c>
-      <c r="K7" s="11">
-        <v>3023</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7">
-        <v>8</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7">
-        <v>1</v>
-      </c>
-      <c r="J8" s="7">
-        <v>1</v>
-      </c>
-      <c r="K8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="D17" s="10">
+        <v>6011</v>
+      </c>
+      <c r="E17" s="10">
+        <v>6012</v>
+      </c>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="C19" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-    </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="10">
-        <v>5000</v>
-      </c>
-      <c r="C12" s="11">
-        <v>5001</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="11">
-        <v>5012</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="11">
-        <v>5033</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7">
-        <v>10</v>
-      </c>
-      <c r="E13" s="7">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7">
-        <v>10</v>
-      </c>
-      <c r="G13" s="7">
-        <v>10</v>
-      </c>
-      <c r="H13" s="7">
-        <v>1</v>
-      </c>
-      <c r="I13" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="C20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3">
-        <v>3</v>
-      </c>
-      <c r="C20" s="3">
-        <v>4</v>
-      </c>
-      <c r="D20" s="3">
-        <v>4</v>
-      </c>
-      <c r="E20" s="3">
-        <v>3</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="16"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated: - Database dump - Database backup - Data memory file
</commit_message>
<xml_diff>
--- a/Tostatura/Doc/DataMemory.xlsx
+++ b/Tostatura/Doc/DataMemory.xlsx
@@ -33,9 +33,6 @@
     <t>NEWALLARME</t>
   </si>
   <si>
-    <t>ALLARMElETTO</t>
-  </si>
-  <si>
     <t>Codice Prodotto Finito</t>
   </si>
   <si>
@@ -151,13 +148,39 @@
   </si>
   <si>
     <t>5034 - 5043</t>
+  </si>
+  <si>
+    <r>
+      <t>ALLARME</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ETTO</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +197,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -322,9 +353,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -342,6 +370,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -652,7 +683,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,22 +702,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="9">
         <v>2990</v>
@@ -706,7 +737,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -726,7 +757,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -740,28 +771,28 @@
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>5</v>
+      <c r="F4" s="19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -774,16 +805,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="9">
         <v>3000</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="10">
         <v>3017</v>
@@ -809,7 +840,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -844,72 +875,72 @@
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="H9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="K9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="G10" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -917,7 +948,7 @@
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="9">
         <v>5000</v>
@@ -926,27 +957,27 @@
         <v>5001</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="10">
         <v>5012</v>
       </c>
       <c r="F12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="H12" s="10">
         <v>5033</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -975,71 +1006,71 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="G14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="I14" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="9">
         <v>6000</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="10">
         <v>6011</v>
@@ -1047,14 +1078,14 @@
       <c r="E17" s="10">
         <v>6012</v>
       </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
@@ -1068,52 +1099,52 @@
       <c r="E18" s="6">
         <v>1</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="E19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="24"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
+        <v>30</v>
+      </c>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C21" s="15"/>

</xml_diff>